<commit_message>
extract data from the research in US
</commit_message>
<xml_diff>
--- a/data/us_news_channel_partisan_score.xlsx
+++ b/data/us_news_channel_partisan_score.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14166\Desktop\BalancedNews\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14166\Desktop\ChromeSamples\BalancedNews\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3513F847-6C42-4DD6-89D4-B9F10379F5ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3F6525-EEDA-4F93-B2F3-925204C2999D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -645,7 +645,7 @@
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>